<commit_message>
changes for cards and level 3 cards
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_3_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_3_CC.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ofoltz\TT\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43686FE2-4B7B-4764-9F0E-382CCF7B1D35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A332DFD5-FFBD-442D-B6B9-0A005BF79772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="26370" windowHeight="15690"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tactile Tabletop Data - Level 3" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="79">
   <si>
     <t>Top Ability Name</t>
   </si>
@@ -103,9 +103,6 @@
     <t>Exhaust</t>
   </si>
   <si>
-    <t>1 Skillpoint</t>
-  </si>
-  <si>
     <t>3 Craftsmanship, 2 Knowledge</t>
   </si>
   <si>
@@ -182,12 +179,93 @@
   </si>
   <si>
     <t>Attack target</t>
+  </si>
+  <si>
+    <t>Turn Warp</t>
+  </si>
+  <si>
+    <t>X = Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lose X life. Take an extra turn after this turn ends and then lose X life again. After taking your extra turn, you must skip your next turn. </t>
+  </si>
+  <si>
+    <t>Extra Steps</t>
+  </si>
+  <si>
+    <t>6 INT</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perform X non-action abilities, and lose 1 life for each one. </t>
+  </si>
+  <si>
+    <t>Organize</t>
+  </si>
+  <si>
+    <t>Decide, layout, and expose the actions for your next turn. Everyone/everything around you knows your next turn. Recover X life, return X cards from discard, and add X to your next roll.</t>
+  </si>
+  <si>
+    <t>Scheme</t>
+  </si>
+  <si>
+    <t xml:space="preserve">During the next round, you may play either of your two actions at any point not during an active turn. At the end of that round, play any actions you have not already. </t>
+  </si>
+  <si>
+    <t>Return to Hand</t>
+  </si>
+  <si>
+    <t>Richochet</t>
+  </si>
+  <si>
+    <t>Near Miss</t>
+  </si>
+  <si>
+    <t>If your attack value does not damage the targeted enemy/enemies, they take X damage.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If your next attack value does not damage a targetted enemy, add X to the attak value and target another enemy in range. Repeat this proces until damage is dealt, or there are no new enemies you can target. </t>
+  </si>
+  <si>
+    <t>Gravity Well</t>
+  </si>
+  <si>
+    <t>Area</t>
+  </si>
+  <si>
+    <t xml:space="preserve">X = Level </t>
+  </si>
+  <si>
+    <t>Inversion</t>
+  </si>
+  <si>
+    <t>Target area 5 feet by 5 feet. All Enemies in and adjacanet to that area cannot move more than 5 feet from targetted area unless they take and suceed an influence check against you.</t>
+  </si>
+  <si>
+    <t>Target area 5 feet by 5 feet. Enemies cannot move within 5 feet of the targetted area unless they make and suceed an influence roll against you.</t>
+  </si>
+  <si>
+    <t>Hookshot</t>
+  </si>
+  <si>
+    <t>Target area within 45 feet and jump to that location</t>
+  </si>
+  <si>
+    <t>Lasso</t>
+  </si>
+  <si>
+    <t>Ally</t>
+  </si>
+  <si>
+    <t>Target Ally within 45 feet and pull them to you.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Touch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1024,12 +1102,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
+    <col min="6" max="6" width="31.140625" customWidth="1"/>
+    <col min="7" max="7" width="21.5703125" customWidth="1"/>
+    <col min="8" max="8" width="22.5703125" customWidth="1"/>
+    <col min="9" max="9" width="22.140625" customWidth="1"/>
+    <col min="10" max="10" width="28.85546875" customWidth="1"/>
+    <col min="11" max="11" width="21.7109375" customWidth="1"/>
+    <col min="12" max="12" width="35.140625" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="32.85546875" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -1115,179 +1211,356 @@
       <c r="L2" t="s">
         <v>25</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>26</v>
-      </c>
-      <c r="N2" t="s">
-        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
       <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>30</v>
-      </c>
-      <c r="E3" t="s">
-        <v>31</v>
       </c>
       <c r="F3" t="s">
         <v>25</v>
       </c>
       <c r="G3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H3" t="s">
         <v>32</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" t="s">
         <v>33</v>
       </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>34</v>
-      </c>
-      <c r="K3" t="s">
-        <v>35</v>
       </c>
       <c r="L3" t="s">
         <v>20</v>
       </c>
-      <c r="M3" t="s">
-        <v>26</v>
-      </c>
       <c r="N3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
+        <v>37</v>
+      </c>
+      <c r="E4" t="s">
         <v>38</v>
-      </c>
-      <c r="E4" t="s">
-        <v>39</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="H4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L4" t="s">
         <v>25</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>42</v>
-      </c>
-      <c r="N4" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E5" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" t="s">
         <v>45</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>46</v>
       </c>
-      <c r="G5" t="s">
-        <v>47</v>
-      </c>
       <c r="H5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I5" t="s">
         <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="K5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L5" t="s">
         <v>20</v>
       </c>
-      <c r="M5" t="s">
-        <v>42</v>
-      </c>
       <c r="N5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="O5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="P5" t="s">
         <v>22</v>
       </c>
       <c r="Q5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="R5" t="s">
+        <v>49</v>
+      </c>
+      <c r="S5" t="s">
+        <v>45</v>
+      </c>
+      <c r="T5" t="s">
         <v>50</v>
       </c>
-      <c r="S5" t="s">
-        <v>46</v>
-      </c>
-      <c r="T5" t="s">
-        <v>51</v>
-      </c>
       <c r="U5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="V5" t="s">
         <v>22</v>
       </c>
       <c r="W5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="X5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Y5" t="s">
         <v>20</v>
       </c>
       <c r="Z5" t="s">
-        <v>42</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6" t="s">
+        <v>53</v>
+      </c>
+      <c r="E6" t="s">
+        <v>54</v>
+      </c>
+      <c r="F6" t="s">
+        <v>25</v>
+      </c>
+      <c r="G6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I6" t="s">
+        <v>22</v>
+      </c>
+      <c r="J6" t="s">
+        <v>53</v>
+      </c>
+      <c r="K6" t="s">
+        <v>57</v>
+      </c>
+      <c r="L6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N6" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" t="s">
+        <v>59</v>
+      </c>
+      <c r="F7" t="s">
+        <v>25</v>
+      </c>
+      <c r="G7" t="s">
+        <v>60</v>
+      </c>
+      <c r="H7" t="s">
+        <v>16</v>
+      </c>
+      <c r="I7" t="s">
+        <v>22</v>
+      </c>
+      <c r="K7" t="s">
+        <v>61</v>
+      </c>
+      <c r="L7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B8" t="s">
+        <v>32</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>53</v>
+      </c>
+      <c r="E8" t="s">
+        <v>66</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>64</v>
+      </c>
+      <c r="H8" t="s">
+        <v>16</v>
+      </c>
+      <c r="I8" t="s">
+        <v>17</v>
+      </c>
+      <c r="J8" t="s">
+        <v>53</v>
+      </c>
+      <c r="K8" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>67</v>
+      </c>
+      <c r="B9" t="s">
+        <v>68</v>
+      </c>
+      <c r="C9" t="s">
+        <v>17</v>
+      </c>
+      <c r="D9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E9" t="s">
+        <v>71</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" t="s">
+        <v>68</v>
+      </c>
+      <c r="I9" t="s">
+        <v>17</v>
+      </c>
+      <c r="J9" t="s">
+        <v>53</v>
+      </c>
+      <c r="K9" t="s">
+        <v>72</v>
+      </c>
+      <c r="L9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>73</v>
+      </c>
+      <c r="B10" t="s">
+        <v>68</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10" t="s">
+        <v>74</v>
+      </c>
+      <c r="F10" t="s">
+        <v>20</v>
+      </c>
+      <c r="G10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" t="s">
+        <v>76</v>
+      </c>
+      <c r="I10" t="s">
+        <v>22</v>
+      </c>
+      <c r="K10" t="s">
+        <v>77</v>
+      </c>
+      <c r="L10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added level 3 cards
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_3_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_3_CC.xlsx
@@ -8,19 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ofoltz\TT\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A332DFD5-FFBD-442D-B6B9-0A005BF79772}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18C6D9D-DE13-414F-BB09-ACD29F5652FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1800" yWindow="4770" windowWidth="52440" windowHeight="25260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tactile Tabletop Data - Level 3" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="144">
   <si>
     <t>Top Ability Name</t>
   </si>
@@ -259,7 +260,202 @@
     <t>Target Ally within 45 feet and pull them to you.</t>
   </si>
   <si>
-    <t xml:space="preserve"> Touch</t>
+    <t>Teamwork</t>
+  </si>
+  <si>
+    <t>Attack    X = Influence</t>
+  </si>
+  <si>
+    <t>Dreamwork</t>
+  </si>
+  <si>
+    <t>If Target Ally helas or buffs you, add X to their value.</t>
+  </si>
+  <si>
+    <t>Take my Hand</t>
+  </si>
+  <si>
+    <t>Choose an ally within 15 feet, they may move to your location. Each of you may now move up to 10 feet.</t>
+  </si>
+  <si>
+    <t>Duplicate</t>
+  </si>
+  <si>
+    <t>Swelling Rage</t>
+  </si>
+  <si>
+    <t>Adrenaline Assault</t>
+  </si>
+  <si>
+    <t>Add X to your attack value. Choose an ally. If they attack the same target you attack with this action during this round, then return this card to your hand from discard and then you each may return one card from discard to your hand.</t>
+  </si>
+  <si>
+    <t>Attack Target Enemy. If an ally attacks that same enemy this round then they add 1d4 to their attacks, and if another ally then attacks that enemy this round they add 2d4 to their attacks, and so on.</t>
+  </si>
+  <si>
+    <t>For this attack, treat 2 handed weapons as 1 handed weapons. You may equipt new weapons for this attack. If required, requipt your original weapons after the attack is finished.</t>
+  </si>
+  <si>
+    <t>Copy targets next action if the action is valid with your equipment and skills.</t>
+  </si>
+  <si>
+    <t>Attack    X = Value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">You and target ally agree to X. If you each deal a combined X or more damage to target enemy this round then that enemy takes an additional X damage. If you and target ally do not deal a combined X or more damage to the target enemy this round then that enemy heals for X. </t>
+  </si>
+  <si>
+    <t>Hand in Hand</t>
+  </si>
+  <si>
+    <t>Common Enemy</t>
+  </si>
+  <si>
+    <t>A target ally may choose to spend one of their actions this round to attack Target Enemy and add their attack value to your attack value.</t>
+  </si>
+  <si>
+    <t>Faithful Watch</t>
+  </si>
+  <si>
+    <t>X = Influence   Y = Level</t>
+  </si>
+  <si>
+    <t>Create a summon on a 5 by 5 space. It has a range of 45 and an attack of X + Y. It's health is equal to your health at the time of casting. Discard a card.</t>
+  </si>
+  <si>
+    <t>Swap</t>
+  </si>
+  <si>
+    <t>Summon</t>
+  </si>
+  <si>
+    <t>Swap places with a target summon. Gain 15 feet of movement</t>
+  </si>
+  <si>
+    <t>Recycle</t>
+  </si>
+  <si>
+    <t>X = Life of Summon</t>
+  </si>
+  <si>
+    <t>Day</t>
+  </si>
+  <si>
+    <t>Destroy target summon you control, disperse X life to the next summon(s) you cast. Heal for X life. Return a card from discard.</t>
+  </si>
+  <si>
+    <t>Comitted</t>
+  </si>
+  <si>
+    <t>X = Life</t>
+  </si>
+  <si>
+    <t>Lose X life, target summon heals for X life.</t>
+  </si>
+  <si>
+    <t>Teleport</t>
+  </si>
+  <si>
+    <t>Target</t>
+  </si>
+  <si>
+    <t>Influence</t>
+  </si>
+  <si>
+    <t>Roll influence if target is unwilling. Teleport target to a surface. Exhaust a card.</t>
+  </si>
+  <si>
+    <t>Respawn</t>
+  </si>
+  <si>
+    <t>Mark area. Teleport to target spot no matter the location</t>
+  </si>
+  <si>
+    <t>5 Rnds</t>
+  </si>
+  <si>
+    <t>Doorway</t>
+  </si>
+  <si>
+    <t>Box</t>
+  </si>
+  <si>
+    <t>3 Rnds</t>
+  </si>
+  <si>
+    <t>Discard a card. Create a 10 x 10 x 10 box over a space. It has 50 hitpoints.</t>
+  </si>
+  <si>
+    <t>Exhaust a card. Summon two doorways. Willing beings can walk through one to come out the other.</t>
+  </si>
+  <si>
+    <t>Push</t>
+  </si>
+  <si>
+    <t>Pull</t>
+  </si>
+  <si>
+    <t>If unwilling roll influence. Pull a target in your direction up to 25 feet.</t>
+  </si>
+  <si>
+    <t>If unwilling roll Influence. Push target up to 25 feet in a direction.</t>
+  </si>
+  <si>
+    <t>Resolve</t>
+  </si>
+  <si>
+    <t>Set your life total to X. You cannot take damage from attacks.</t>
+  </si>
+  <si>
+    <t>2 Rnds</t>
+  </si>
+  <si>
+    <t>Heroic Defense</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Double all Defense Values. You cannot make an attack. </t>
+  </si>
+  <si>
+    <t>Limit Break</t>
+  </si>
+  <si>
+    <t>Increase either an attack die or defense die of one of your equipped weapons, and then decrease one opposite die. (d4 -&gt; d2, d2 -&gt; 0)</t>
+  </si>
+  <si>
+    <t>Craftsman Work</t>
+  </si>
+  <si>
+    <t>Self/Ally</t>
+  </si>
+  <si>
+    <t>Target equipped weapon. It gets +1 to all Rolls.</t>
+  </si>
+  <si>
+    <t>Predator</t>
+  </si>
+  <si>
+    <t>At the beginning of each of your turns, mark target enemy</t>
+  </si>
+  <si>
+    <t>Ambush</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Remove mark from target enemy. Gain 20 feet of movement. Play two additional actions this turn. </t>
+  </si>
+  <si>
+    <t>Soothing Touch</t>
+  </si>
+  <si>
+    <t>Ally/Self</t>
+  </si>
+  <si>
+    <t>Heal adjacent Targets up to X hitpoints each</t>
+  </si>
+  <si>
+    <t>Give Haste</t>
+  </si>
+  <si>
+    <t>While Active you can only play one action per turn, and target ally can play one additional action per turn.</t>
   </si>
 </sst>
 </file>
@@ -1103,10 +1299,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Z23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1174,7 +1370,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1561,6 +1757,468 @@
     <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>78</v>
+      </c>
+      <c r="B11" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>79</v>
+      </c>
+      <c r="E11" t="s">
+        <v>87</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" t="s">
+        <v>76</v>
+      </c>
+      <c r="I11" t="s">
+        <v>17</v>
+      </c>
+      <c r="J11" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" t="s">
+        <v>81</v>
+      </c>
+      <c r="L11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>82</v>
+      </c>
+      <c r="B12" t="s">
+        <v>76</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12" t="s">
+        <v>83</v>
+      </c>
+      <c r="F12" t="s">
+        <v>20</v>
+      </c>
+      <c r="G12" t="s">
+        <v>84</v>
+      </c>
+      <c r="H12" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" t="s">
+        <v>90</v>
+      </c>
+      <c r="L12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>85</v>
+      </c>
+      <c r="B13" t="s">
+        <v>32</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" t="s">
+        <v>88</v>
+      </c>
+      <c r="F13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" t="s">
+        <v>86</v>
+      </c>
+      <c r="H13" t="s">
+        <v>32</v>
+      </c>
+      <c r="I13" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" t="s">
+        <v>33</v>
+      </c>
+      <c r="K13" t="s">
+        <v>89</v>
+      </c>
+      <c r="L13" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14" t="s">
+        <v>91</v>
+      </c>
+      <c r="E14" t="s">
+        <v>92</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>94</v>
+      </c>
+      <c r="H14" t="s">
+        <v>32</v>
+      </c>
+      <c r="I14" t="s">
+        <v>22</v>
+      </c>
+      <c r="J14" t="s">
+        <v>33</v>
+      </c>
+      <c r="K14" t="s">
+        <v>95</v>
+      </c>
+      <c r="L14" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>96</v>
+      </c>
+      <c r="B15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C15" t="s">
+        <v>17</v>
+      </c>
+      <c r="D15" t="s">
+        <v>97</v>
+      </c>
+      <c r="E15" t="s">
+        <v>98</v>
+      </c>
+      <c r="F15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G15" t="s">
+        <v>99</v>
+      </c>
+      <c r="H15" t="s">
+        <v>100</v>
+      </c>
+      <c r="I15" t="s">
+        <v>22</v>
+      </c>
+      <c r="K15" t="s">
+        <v>101</v>
+      </c>
+      <c r="L15" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>102</v>
+      </c>
+      <c r="B16" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" t="s">
+        <v>22</v>
+      </c>
+      <c r="D16" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" t="s">
+        <v>105</v>
+      </c>
+      <c r="F16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G16" t="s">
+        <v>106</v>
+      </c>
+      <c r="H16" t="s">
+        <v>100</v>
+      </c>
+      <c r="I16" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" t="s">
+        <v>107</v>
+      </c>
+      <c r="K16" t="s">
+        <v>108</v>
+      </c>
+      <c r="L16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>109</v>
+      </c>
+      <c r="B17" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17" t="s">
+        <v>111</v>
+      </c>
+      <c r="E17" t="s">
+        <v>112</v>
+      </c>
+      <c r="F17" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" t="s">
+        <v>113</v>
+      </c>
+      <c r="H17" t="s">
+        <v>68</v>
+      </c>
+      <c r="I17" t="s">
+        <v>104</v>
+      </c>
+      <c r="K17" t="s">
+        <v>114</v>
+      </c>
+      <c r="L17" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>116</v>
+      </c>
+      <c r="C18" t="s">
+        <v>115</v>
+      </c>
+      <c r="E18" t="s">
+        <v>120</v>
+      </c>
+      <c r="F18" t="s">
+        <v>20</v>
+      </c>
+      <c r="G18" t="s">
+        <v>117</v>
+      </c>
+      <c r="H18" t="s">
+        <v>68</v>
+      </c>
+      <c r="I18" t="s">
+        <v>118</v>
+      </c>
+      <c r="K18" t="s">
+        <v>119</v>
+      </c>
+      <c r="L18" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>121</v>
+      </c>
+      <c r="B19" t="s">
+        <v>110</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19" t="s">
+        <v>111</v>
+      </c>
+      <c r="E19" t="s">
+        <v>124</v>
+      </c>
+      <c r="F19" t="s">
+        <v>20</v>
+      </c>
+      <c r="G19" t="s">
+        <v>122</v>
+      </c>
+      <c r="H19" t="s">
+        <v>110</v>
+      </c>
+      <c r="I19" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" t="s">
+        <v>111</v>
+      </c>
+      <c r="K19" t="s">
+        <v>123</v>
+      </c>
+      <c r="L19" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>125</v>
+      </c>
+      <c r="B20" t="s">
+        <v>16</v>
+      </c>
+      <c r="C20" t="s">
+        <v>127</v>
+      </c>
+      <c r="D20" t="s">
+        <v>53</v>
+      </c>
+      <c r="E20" t="s">
+        <v>126</v>
+      </c>
+      <c r="F20" t="s">
+        <v>25</v>
+      </c>
+      <c r="G20" t="s">
+        <v>128</v>
+      </c>
+      <c r="H20" t="s">
+        <v>16</v>
+      </c>
+      <c r="I20" t="s">
+        <v>127</v>
+      </c>
+      <c r="K20" t="s">
+        <v>129</v>
+      </c>
+      <c r="L20" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>130</v>
+      </c>
+      <c r="B21" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" t="s">
+        <v>17</v>
+      </c>
+      <c r="D21" t="s">
+        <v>53</v>
+      </c>
+      <c r="E21" t="s">
+        <v>131</v>
+      </c>
+      <c r="F21" t="s">
+        <v>20</v>
+      </c>
+      <c r="G21" t="s">
+        <v>132</v>
+      </c>
+      <c r="H21" t="s">
+        <v>133</v>
+      </c>
+      <c r="I21" t="s">
+        <v>17</v>
+      </c>
+      <c r="J21" t="s">
+        <v>53</v>
+      </c>
+      <c r="K21" t="s">
+        <v>134</v>
+      </c>
+      <c r="L21" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>135</v>
+      </c>
+      <c r="B22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C22" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" t="s">
+        <v>53</v>
+      </c>
+      <c r="E22" t="s">
+        <v>136</v>
+      </c>
+      <c r="F22" t="s">
+        <v>20</v>
+      </c>
+      <c r="G22" t="s">
+        <v>137</v>
+      </c>
+      <c r="H22" t="s">
+        <v>32</v>
+      </c>
+      <c r="I22" t="s">
+        <v>22</v>
+      </c>
+      <c r="K22" t="s">
+        <v>138</v>
+      </c>
+      <c r="L22" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>139</v>
+      </c>
+      <c r="B23" t="s">
+        <v>140</v>
+      </c>
+      <c r="C23" t="s">
+        <v>22</v>
+      </c>
+      <c r="D23" t="s">
+        <v>29</v>
+      </c>
+      <c r="E23" t="s">
+        <v>141</v>
+      </c>
+      <c r="F23" t="s">
+        <v>25</v>
+      </c>
+      <c r="G23" t="s">
+        <v>142</v>
+      </c>
+      <c r="H23" t="s">
+        <v>76</v>
+      </c>
+      <c r="I23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J23" t="s">
+        <v>53</v>
+      </c>
+      <c r="K23" t="s">
+        <v>143</v>
+      </c>
+      <c r="L23" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
assigned points to level 3 cards, moved some level 3 cards to level 4
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_3_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_3_CC.xlsx
@@ -8,20 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ofoltz\TT\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C18C6D9D-DE13-414F-BB09-ACD29F5652FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D1ADCF-B766-47B6-A430-0CCB64FBC68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1800" yWindow="4770" windowWidth="52440" windowHeight="25260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tactile Tabletop Data - Level 3" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="127">
   <si>
     <t>Top Ability Name</t>
   </si>
@@ -104,9 +103,6 @@
     <t>Exhaust</t>
   </si>
   <si>
-    <t>3 Craftsmanship, 2 Knowledge</t>
-  </si>
-  <si>
     <t>Well of Life</t>
   </si>
   <si>
@@ -116,9 +112,6 @@
     <t>X = Influence</t>
   </si>
   <si>
-    <t>Action can only be used by itself. At start of next turn, recover all discarded cards, Heal for X, and add X to defence die for 1 rnd</t>
-  </si>
-  <si>
     <t>Guided Strike</t>
   </si>
   <si>
@@ -131,57 +124,18 @@
     <t>Attack target once this turn, again at start of next turn</t>
   </si>
   <si>
-    <t>2 Spirituality, 3 Charisma</t>
-  </si>
-  <si>
     <t>Neck Cracker</t>
   </si>
   <si>
     <t>Attack    X = Level</t>
   </si>
   <si>
-    <t>Make an Unarmed attack, add X to the Attack Value. If you deal damage Attack Target Enemy. Target Enemy cannot use movement on their next turn.</t>
-  </si>
-  <si>
     <t>Shatter Weapon</t>
   </si>
   <si>
-    <t>Make an Unarmed attack against an enemy and add X to the Attack Value.Lose X life. If you deal damage, you may choose to destroy one of their equipped weapons</t>
-  </si>
-  <si>
-    <t>1 Health</t>
-  </si>
-  <si>
-    <t>4 STR and 2 VIG</t>
-  </si>
-  <si>
-    <t>Lightning Strike</t>
-  </si>
-  <si>
-    <t>Attack Target Enemy twice and add X to each Attack Value. Discard a card.</t>
-  </si>
-  <si>
     <t>Hand</t>
   </si>
   <si>
-    <t>Reliable Strike</t>
-  </si>
-  <si>
-    <t>Attack target, add X to your Attack Value. If no damage is dealt then return this card to your hand.</t>
-  </si>
-  <si>
-    <t>Quick Strike</t>
-  </si>
-  <si>
-    <t>Discard a card</t>
-  </si>
-  <si>
-    <t>Basic Strike</t>
-  </si>
-  <si>
-    <t>Attack target</t>
-  </si>
-  <si>
     <t>Turn Warp</t>
   </si>
   <si>
@@ -194,12 +148,6 @@
     <t>Extra Steps</t>
   </si>
   <si>
-    <t>6 INT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Perform X non-action abilities, and lose 1 life for each one. </t>
-  </si>
-  <si>
     <t>Organize</t>
   </si>
   <si>
@@ -215,18 +163,6 @@
     <t>Return to Hand</t>
   </si>
   <si>
-    <t>Richochet</t>
-  </si>
-  <si>
-    <t>Near Miss</t>
-  </si>
-  <si>
-    <t>If your attack value does not damage the targeted enemy/enemies, they take X damage.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If your next attack value does not damage a targetted enemy, add X to the attak value and target another enemy in range. Repeat this proces until damage is dealt, or there are no new enemies you can target. </t>
-  </si>
-  <si>
     <t>Gravity Well</t>
   </si>
   <si>
@@ -239,39 +175,21 @@
     <t>Inversion</t>
   </si>
   <si>
-    <t>Target area 5 feet by 5 feet. All Enemies in and adjacanet to that area cannot move more than 5 feet from targetted area unless they take and suceed an influence check against you.</t>
-  </si>
-  <si>
-    <t>Target area 5 feet by 5 feet. Enemies cannot move within 5 feet of the targetted area unless they make and suceed an influence roll against you.</t>
-  </si>
-  <si>
     <t>Hookshot</t>
   </si>
   <si>
-    <t>Target area within 45 feet and jump to that location</t>
-  </si>
-  <si>
     <t>Lasso</t>
   </si>
   <si>
     <t>Ally</t>
   </si>
   <si>
-    <t>Target Ally within 45 feet and pull them to you.</t>
-  </si>
-  <si>
     <t>Teamwork</t>
   </si>
   <si>
-    <t>Attack    X = Influence</t>
-  </si>
-  <si>
     <t>Dreamwork</t>
   </si>
   <si>
-    <t>If Target Ally helas or buffs you, add X to their value.</t>
-  </si>
-  <si>
     <t>Take my Hand</t>
   </si>
   <si>
@@ -281,39 +199,6 @@
     <t>Duplicate</t>
   </si>
   <si>
-    <t>Swelling Rage</t>
-  </si>
-  <si>
-    <t>Adrenaline Assault</t>
-  </si>
-  <si>
-    <t>Add X to your attack value. Choose an ally. If they attack the same target you attack with this action during this round, then return this card to your hand from discard and then you each may return one card from discard to your hand.</t>
-  </si>
-  <si>
-    <t>Attack Target Enemy. If an ally attacks that same enemy this round then they add 1d4 to their attacks, and if another ally then attacks that enemy this round they add 2d4 to their attacks, and so on.</t>
-  </si>
-  <si>
-    <t>For this attack, treat 2 handed weapons as 1 handed weapons. You may equipt new weapons for this attack. If required, requipt your original weapons after the attack is finished.</t>
-  </si>
-  <si>
-    <t>Copy targets next action if the action is valid with your equipment and skills.</t>
-  </si>
-  <si>
-    <t>Attack    X = Value</t>
-  </si>
-  <si>
-    <t xml:space="preserve">You and target ally agree to X. If you each deal a combined X or more damage to target enemy this round then that enemy takes an additional X damage. If you and target ally do not deal a combined X or more damage to the target enemy this round then that enemy heals for X. </t>
-  </si>
-  <si>
-    <t>Hand in Hand</t>
-  </si>
-  <si>
-    <t>Common Enemy</t>
-  </si>
-  <si>
-    <t>A target ally may choose to spend one of their actions this round to attack Target Enemy and add their attack value to your attack value.</t>
-  </si>
-  <si>
     <t>Faithful Watch</t>
   </si>
   <si>
@@ -456,6 +341,69 @@
   </si>
   <si>
     <t>While Active you can only play one action per turn, and target ally can play one additional action per turn.</t>
+  </si>
+  <si>
+    <t>Only this action can be played this turn. At start of next turn, recover all discarded cards, heal for X, and add X to defence values</t>
+  </si>
+  <si>
+    <t>2 Strength, 2 Knowledge, 3 Vigor</t>
+  </si>
+  <si>
+    <t>Make an Unarmed attack, add X to the Attack Value. If you deal damage Attack Target Enemy again. Target Enemy cannot use movement on their next turn.</t>
+  </si>
+  <si>
+    <t>Make an Unarmed attack against an enemy. Lose X life. If you deal damage, you may choose to destroy one of their equipped weapons</t>
+  </si>
+  <si>
+    <t>2 Charisma, 5 Strength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Perform X non-action abilities, and lose 1 life for each one taken. </t>
+  </si>
+  <si>
+    <t>7 Knowledge</t>
+  </si>
+  <si>
+    <t>5 Knowledge, 2 Vigor</t>
+  </si>
+  <si>
+    <t>Target area 5 feet by 5 feet. All Enemies in and adjacanet to that area cannot move more than 5 feet from targetted area unless they take and succeed an influence check against you.</t>
+  </si>
+  <si>
+    <t>Target area 5 feet by 5 feet. Enemies cannot move onto or adjacent to the targetted area unless they make and succeed an influence roll against you.</t>
+  </si>
+  <si>
+    <t>Target 5 x 5 foot area within 45 feet and jump to that location</t>
+  </si>
+  <si>
+    <t>Target Ally within 45 feet and pull them adjacent to you.</t>
+  </si>
+  <si>
+    <t>3 Charisma, 4 Craftsmanship</t>
+  </si>
+  <si>
+    <t>1 Perception, 2 Vigor, 3 Finesse, 1 Knowledge</t>
+  </si>
+  <si>
+    <t>4 Finesse, 3 Charisma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attack </t>
+  </si>
+  <si>
+    <t>Choose an ally. Attack Target enemy. If they attack the same target you attack with this action during this round, then return this card to your hand from discard and then you each may return one card from discard to your hand.</t>
+  </si>
+  <si>
+    <t>If Target Ally heals or buffs you, add X to their value.</t>
+  </si>
+  <si>
+    <t>5 Spirituality, 2 Knowledge</t>
+  </si>
+  <si>
+    <t>Copy targets next action if the action is valid with your equipment and skills, and then play it after targets turn ends.</t>
+  </si>
+  <si>
+    <t>4 Charisma, 3 Knowledge</t>
   </si>
 </sst>
 </file>
@@ -1299,31 +1247,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z23"/>
+  <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" customWidth="1"/>
-    <col min="3" max="3" width="19.42578125" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
     <col min="4" max="4" width="25.7109375" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="31.140625" customWidth="1"/>
+    <col min="5" max="5" width="169.5703125" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
     <col min="7" max="7" width="21.5703125" customWidth="1"/>
-    <col min="8" max="8" width="22.5703125" customWidth="1"/>
-    <col min="9" max="9" width="22.140625" customWidth="1"/>
-    <col min="10" max="10" width="28.85546875" customWidth="1"/>
-    <col min="11" max="11" width="21.7109375" customWidth="1"/>
-    <col min="12" max="12" width="35.140625" customWidth="1"/>
+    <col min="8" max="8" width="11.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" customWidth="1"/>
+    <col min="10" max="10" width="37" customWidth="1"/>
+    <col min="11" max="11" width="138.42578125" customWidth="1"/>
+    <col min="12" max="12" width="20.7109375" customWidth="1"/>
     <col min="13" max="13" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="32.85546875" customWidth="1"/>
+    <col min="14" max="14" width="39.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1370,7 +1318,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:26" ht="135" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" ht="135" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>15</v>
       </c>
@@ -1408,171 +1356,135 @@
         <v>25</v>
       </c>
       <c r="N2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>26</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>27</v>
       </c>
       <c r="B3" t="s">
         <v>16</v>
       </c>
       <c r="C3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" t="s">
-        <v>29</v>
-      </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>106</v>
       </c>
       <c r="F3" t="s">
         <v>25</v>
       </c>
       <c r="G3" t="s">
+        <v>29</v>
+      </c>
+      <c r="H3" t="s">
+        <v>30</v>
+      </c>
+      <c r="I3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
         <v>31</v>
       </c>
-      <c r="H3" t="s">
+      <c r="K3" t="s">
         <v>32</v>
       </c>
-      <c r="I3" t="s">
-        <v>28</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="L3" t="s">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>33</v>
       </c>
-      <c r="K3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" t="s">
-        <v>20</v>
-      </c>
-      <c r="N3" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>36</v>
-      </c>
       <c r="B4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C4" t="s">
         <v>22</v>
       </c>
       <c r="D4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>38</v>
+        <v>108</v>
       </c>
       <c r="F4" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="G4" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="H4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="I4" t="s">
         <v>22</v>
       </c>
       <c r="J4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
       <c r="L4" t="s">
         <v>25</v>
       </c>
       <c r="N4" t="s">
-        <v>42</v>
+        <v>110</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B5" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="C5" t="s">
         <v>22</v>
       </c>
       <c r="D5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="E5" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="F5" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="G5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
+        <v>16</v>
       </c>
       <c r="I5" t="s">
         <v>22</v>
       </c>
       <c r="J5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>47</v>
+        <v>111</v>
       </c>
       <c r="L5" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="N5" t="s">
-        <v>48</v>
-      </c>
-      <c r="O5" t="s">
-        <v>32</v>
-      </c>
-      <c r="P5" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>33</v>
-      </c>
-      <c r="R5" t="s">
-        <v>49</v>
-      </c>
-      <c r="S5" t="s">
-        <v>45</v>
-      </c>
-      <c r="T5" t="s">
-        <v>50</v>
-      </c>
-      <c r="U5" t="s">
-        <v>32</v>
-      </c>
-      <c r="V5" t="s">
-        <v>22</v>
-      </c>
-      <c r="W5" t="s">
-        <v>33</v>
-      </c>
-      <c r="X5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>20</v>
-      </c>
-      <c r="Z5" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>52</v>
       </c>
       <c r="B6" t="s">
         <v>16</v>
@@ -1581,16 +1493,16 @@
         <v>22</v>
       </c>
       <c r="D6" t="s">
-        <v>53</v>
+        <v>38</v>
       </c>
       <c r="E6" t="s">
-        <v>54</v>
+        <v>42</v>
       </c>
       <c r="F6" t="s">
         <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
       <c r="H6" t="s">
         <v>16</v>
@@ -1598,376 +1510,373 @@
       <c r="I6" t="s">
         <v>22</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L6" t="s">
+        <v>45</v>
+      </c>
+      <c r="N6" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" t="s">
+        <v>48</v>
+      </c>
+      <c r="E7" t="s">
+        <v>114</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>49</v>
+      </c>
+      <c r="H7" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" t="s">
+        <v>17</v>
+      </c>
+      <c r="J7" t="s">
+        <v>38</v>
+      </c>
+      <c r="K7" t="s">
+        <v>115</v>
+      </c>
+      <c r="L7" t="s">
+        <v>20</v>
+      </c>
+      <c r="N7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="E8" t="s">
+        <v>116</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8" t="s">
+        <v>51</v>
+      </c>
+      <c r="H8" t="s">
+        <v>52</v>
+      </c>
+      <c r="I8" t="s">
+        <v>22</v>
+      </c>
+      <c r="K8" t="s">
+        <v>117</v>
+      </c>
+      <c r="L8" t="s">
+        <v>20</v>
+      </c>
+      <c r="N8" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>53</v>
       </c>
-      <c r="K6" t="s">
-        <v>57</v>
-      </c>
-      <c r="L6" t="s">
-        <v>25</v>
-      </c>
-      <c r="N6" t="s">
-        <v>56</v>
+      <c r="B9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" t="s">
+        <v>22</v>
+      </c>
+      <c r="D9" t="s">
+        <v>121</v>
+      </c>
+      <c r="E9" t="s">
+        <v>122</v>
+      </c>
+      <c r="F9" t="s">
+        <v>20</v>
+      </c>
+      <c r="G9" t="s">
+        <v>54</v>
+      </c>
+      <c r="H9" t="s">
+        <v>52</v>
+      </c>
+      <c r="I9" t="s">
+        <v>27</v>
+      </c>
+      <c r="J9" t="s">
+        <v>38</v>
+      </c>
+      <c r="K9" t="s">
+        <v>123</v>
+      </c>
+      <c r="L9" t="s">
+        <v>36</v>
+      </c>
+      <c r="N9" t="s">
+        <v>124</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>58</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E7" t="s">
-        <v>59</v>
-      </c>
-      <c r="F7" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" t="s">
-        <v>60</v>
-      </c>
-      <c r="H7" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" t="s">
-        <v>22</v>
-      </c>
-      <c r="K7" t="s">
-        <v>61</v>
-      </c>
-      <c r="L7" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B8" t="s">
-        <v>32</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8" t="s">
-        <v>64</v>
-      </c>
-      <c r="H8" t="s">
-        <v>16</v>
-      </c>
-      <c r="I8" t="s">
-        <v>17</v>
-      </c>
-      <c r="J8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K8" t="s">
-        <v>65</v>
-      </c>
-      <c r="L8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>67</v>
-      </c>
-      <c r="B9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C9" t="s">
-        <v>17</v>
-      </c>
-      <c r="D9" t="s">
-        <v>69</v>
-      </c>
-      <c r="E9" t="s">
-        <v>71</v>
-      </c>
-      <c r="F9" t="s">
-        <v>20</v>
-      </c>
-      <c r="G9" t="s">
-        <v>70</v>
-      </c>
-      <c r="H9" t="s">
-        <v>68</v>
-      </c>
-      <c r="I9" t="s">
-        <v>17</v>
-      </c>
-      <c r="J9" t="s">
-        <v>53</v>
-      </c>
-      <c r="K9" t="s">
-        <v>72</v>
-      </c>
-      <c r="L9" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>73</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>52</v>
       </c>
       <c r="C10" t="s">
         <v>22</v>
       </c>
       <c r="E10" t="s">
-        <v>74</v>
+        <v>56</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
       </c>
       <c r="G10" t="s">
-        <v>75</v>
+        <v>57</v>
       </c>
       <c r="H10" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="I10" t="s">
+        <v>27</v>
+      </c>
+      <c r="K10" t="s">
+        <v>125</v>
+      </c>
+      <c r="L10" t="s">
+        <v>36</v>
+      </c>
+      <c r="N10" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>58</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E11" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>61</v>
+      </c>
+      <c r="H11" t="s">
+        <v>62</v>
+      </c>
+      <c r="I11" t="s">
         <v>22</v>
       </c>
-      <c r="K10" t="s">
-        <v>77</v>
-      </c>
-      <c r="L10" t="s">
+      <c r="K11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L11" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>78</v>
-      </c>
-      <c r="B11" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E11" t="s">
-        <v>87</v>
-      </c>
-      <c r="F11" t="s">
-        <v>20</v>
-      </c>
-      <c r="G11" t="s">
-        <v>80</v>
-      </c>
-      <c r="H11" t="s">
-        <v>76</v>
-      </c>
-      <c r="I11" t="s">
-        <v>17</v>
-      </c>
-      <c r="J11" t="s">
-        <v>53</v>
-      </c>
-      <c r="K11" t="s">
-        <v>81</v>
-      </c>
-      <c r="L11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="C12" t="s">
         <v>22</v>
       </c>
+      <c r="D12" t="s">
+        <v>65</v>
+      </c>
       <c r="E12" t="s">
-        <v>83</v>
+        <v>67</v>
       </c>
       <c r="F12" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="H12" t="s">
-        <v>76</v>
+        <v>62</v>
       </c>
       <c r="I12" t="s">
-        <v>28</v>
+        <v>22</v>
+      </c>
+      <c r="J12" t="s">
+        <v>69</v>
       </c>
       <c r="K12" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="L12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>85</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>32</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>33</v>
+        <v>73</v>
       </c>
       <c r="E13" t="s">
-        <v>88</v>
+        <v>74</v>
       </c>
       <c r="F13" t="s">
+        <v>20</v>
+      </c>
+      <c r="G13" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" t="s">
+        <v>66</v>
+      </c>
+      <c r="K13" t="s">
+        <v>76</v>
+      </c>
+      <c r="L13" t="s">
         <v>25</v>
       </c>
-      <c r="G13" t="s">
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" t="s">
+        <v>77</v>
+      </c>
+      <c r="E14" t="s">
+        <v>82</v>
+      </c>
+      <c r="F14" t="s">
+        <v>20</v>
+      </c>
+      <c r="G14" t="s">
+        <v>79</v>
+      </c>
+      <c r="H14" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K14" t="s">
+        <v>81</v>
+      </c>
+      <c r="L14" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C15" t="s">
+        <v>22</v>
+      </c>
+      <c r="D15" t="s">
+        <v>73</v>
+      </c>
+      <c r="E15" t="s">
         <v>86</v>
       </c>
-      <c r="H13" t="s">
-        <v>32</v>
-      </c>
-      <c r="I13" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" t="s">
-        <v>33</v>
-      </c>
-      <c r="K13" t="s">
-        <v>89</v>
-      </c>
-      <c r="L13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>93</v>
-      </c>
-      <c r="B14" t="s">
-        <v>32</v>
-      </c>
-      <c r="C14" t="s">
-        <v>22</v>
-      </c>
-      <c r="D14" t="s">
-        <v>91</v>
-      </c>
-      <c r="E14" t="s">
-        <v>92</v>
-      </c>
-      <c r="F14" t="s">
-        <v>20</v>
-      </c>
-      <c r="G14" t="s">
-        <v>94</v>
-      </c>
-      <c r="H14" t="s">
-        <v>32</v>
-      </c>
-      <c r="I14" t="s">
-        <v>22</v>
-      </c>
-      <c r="J14" t="s">
-        <v>33</v>
-      </c>
-      <c r="K14" t="s">
-        <v>95</v>
-      </c>
-      <c r="L14" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>96</v>
-      </c>
-      <c r="B15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C15" t="s">
-        <v>17</v>
-      </c>
-      <c r="D15" t="s">
-        <v>97</v>
-      </c>
-      <c r="E15" t="s">
-        <v>98</v>
-      </c>
       <c r="F15" t="s">
         <v>20</v>
       </c>
       <c r="G15" t="s">
-        <v>99</v>
+        <v>84</v>
       </c>
       <c r="H15" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
       <c r="I15" t="s">
         <v>22</v>
       </c>
+      <c r="J15" t="s">
+        <v>73</v>
+      </c>
       <c r="K15" t="s">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="L15" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>102</v>
+        <v>87</v>
       </c>
       <c r="B16" t="s">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>22</v>
+        <v>89</v>
       </c>
       <c r="D16" t="s">
-        <v>103</v>
+        <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>105</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
         <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>106</v>
+        <v>90</v>
       </c>
       <c r="H16" t="s">
-        <v>100</v>
+        <v>16</v>
       </c>
       <c r="I16" t="s">
-        <v>22</v>
-      </c>
-      <c r="J16" t="s">
-        <v>107</v>
+        <v>89</v>
       </c>
       <c r="K16" t="s">
-        <v>108</v>
+        <v>91</v>
       </c>
       <c r="L16" t="s">
         <v>20</v>
@@ -1975,249 +1884,112 @@
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="B17" t="s">
-        <v>110</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D17" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>112</v>
+        <v>93</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
       </c>
       <c r="G17" t="s">
-        <v>113</v>
+        <v>94</v>
       </c>
       <c r="H17" t="s">
-        <v>68</v>
+        <v>95</v>
       </c>
       <c r="I17" t="s">
-        <v>104</v>
+        <v>17</v>
+      </c>
+      <c r="J17" t="s">
+        <v>38</v>
       </c>
       <c r="K17" t="s">
-        <v>114</v>
+        <v>96</v>
       </c>
       <c r="L17" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>116</v>
+        <v>97</v>
+      </c>
+      <c r="B18" t="s">
+        <v>30</v>
       </c>
       <c r="C18" t="s">
-        <v>115</v>
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>120</v>
+        <v>98</v>
       </c>
       <c r="F18" t="s">
         <v>20</v>
       </c>
       <c r="G18" t="s">
-        <v>117</v>
+        <v>99</v>
       </c>
       <c r="H18" t="s">
-        <v>68</v>
+        <v>30</v>
       </c>
       <c r="I18" t="s">
-        <v>118</v>
+        <v>22</v>
       </c>
       <c r="K18" t="s">
-        <v>119</v>
+        <v>100</v>
       </c>
       <c r="L18" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>121</v>
+        <v>101</v>
       </c>
       <c r="B19" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
       </c>
       <c r="D19" t="s">
-        <v>111</v>
+        <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>124</v>
+        <v>103</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G19" t="s">
-        <v>122</v>
+        <v>104</v>
       </c>
       <c r="H19" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="I19" t="s">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="J19" t="s">
-        <v>111</v>
+        <v>38</v>
       </c>
       <c r="K19" t="s">
-        <v>123</v>
+        <v>105</v>
       </c>
       <c r="L19" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>125</v>
-      </c>
-      <c r="B20" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" t="s">
-        <v>127</v>
-      </c>
-      <c r="D20" t="s">
-        <v>53</v>
-      </c>
-      <c r="E20" t="s">
-        <v>126</v>
-      </c>
-      <c r="F20" t="s">
-        <v>25</v>
-      </c>
-      <c r="G20" t="s">
-        <v>128</v>
-      </c>
-      <c r="H20" t="s">
-        <v>16</v>
-      </c>
-      <c r="I20" t="s">
-        <v>127</v>
-      </c>
-      <c r="K20" t="s">
-        <v>129</v>
-      </c>
-      <c r="L20" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>130</v>
-      </c>
-      <c r="B21" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" t="s">
-        <v>17</v>
-      </c>
-      <c r="D21" t="s">
-        <v>53</v>
-      </c>
-      <c r="E21" t="s">
-        <v>131</v>
-      </c>
-      <c r="F21" t="s">
-        <v>20</v>
-      </c>
-      <c r="G21" t="s">
-        <v>132</v>
-      </c>
-      <c r="H21" t="s">
-        <v>133</v>
-      </c>
-      <c r="I21" t="s">
-        <v>17</v>
-      </c>
-      <c r="J21" t="s">
-        <v>53</v>
-      </c>
-      <c r="K21" t="s">
-        <v>134</v>
-      </c>
-      <c r="L21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>135</v>
-      </c>
-      <c r="B22" t="s">
-        <v>32</v>
-      </c>
-      <c r="C22" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" t="s">
-        <v>53</v>
-      </c>
-      <c r="E22" t="s">
-        <v>136</v>
-      </c>
-      <c r="F22" t="s">
-        <v>20</v>
-      </c>
-      <c r="G22" t="s">
-        <v>137</v>
-      </c>
-      <c r="H22" t="s">
-        <v>32</v>
-      </c>
-      <c r="I22" t="s">
-        <v>22</v>
-      </c>
-      <c r="K22" t="s">
-        <v>138</v>
-      </c>
-      <c r="L22" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>139</v>
-      </c>
-      <c r="B23" t="s">
-        <v>140</v>
-      </c>
-      <c r="C23" t="s">
-        <v>22</v>
-      </c>
-      <c r="D23" t="s">
-        <v>29</v>
-      </c>
-      <c r="E23" t="s">
-        <v>141</v>
-      </c>
-      <c r="F23" t="s">
-        <v>25</v>
-      </c>
-      <c r="G23" t="s">
-        <v>142</v>
-      </c>
-      <c r="H23" t="s">
-        <v>76</v>
-      </c>
-      <c r="I23" t="s">
-        <v>17</v>
-      </c>
-      <c r="J23" t="s">
-        <v>53</v>
-      </c>
-      <c r="K23" t="s">
-        <v>143</v>
-      </c>
-      <c r="L23" t="s">
         <v>20</v>
       </c>
     </row>

</xml_diff>

<commit_message>
checked level 3 skill points
</commit_message>
<xml_diff>
--- a/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_3_CC.xlsx
+++ b/tactile_tabletop/Character Cards/Tactile_Tabletop_Data-Level_3_CC.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ofoltz\TT\TableTopRolePlaying_Squib\tactile_tabletop\Character Cards\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D1ADCF-B766-47B6-A430-0CCB64FBC68A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AF62364-BD78-4369-8F74-C1EF30E45F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="57840" windowHeight="32190" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="136">
   <si>
     <t>Top Ability Name</t>
   </si>
@@ -226,9 +226,6 @@
     <t>Day</t>
   </si>
   <si>
-    <t>Destroy target summon you control, disperse X life to the next summon(s) you cast. Heal for X life. Return a card from discard.</t>
-  </si>
-  <si>
     <t>Comitted</t>
   </si>
   <si>
@@ -247,15 +244,9 @@
     <t>Influence</t>
   </si>
   <si>
-    <t>Roll influence if target is unwilling. Teleport target to a surface. Exhaust a card.</t>
-  </si>
-  <si>
     <t>Respawn</t>
   </si>
   <si>
-    <t>Mark area. Teleport to target spot no matter the location</t>
-  </si>
-  <si>
     <t>5 Rnds</t>
   </si>
   <si>
@@ -268,9 +259,6 @@
     <t>3 Rnds</t>
   </si>
   <si>
-    <t>Discard a card. Create a 10 x 10 x 10 box over a space. It has 50 hitpoints.</t>
-  </si>
-  <si>
     <t>Exhaust a card. Summon two doorways. Willing beings can walk through one to come out the other.</t>
   </si>
   <si>
@@ -304,9 +292,6 @@
     <t>Limit Break</t>
   </si>
   <si>
-    <t>Increase either an attack die or defense die of one of your equipped weapons, and then decrease one opposite die. (d4 -&gt; d2, d2 -&gt; 0)</t>
-  </si>
-  <si>
     <t>Craftsman Work</t>
   </si>
   <si>
@@ -373,9 +358,6 @@
     <t>Target area 5 feet by 5 feet. Enemies cannot move onto or adjacent to the targetted area unless they make and succeed an influence roll against you.</t>
   </si>
   <si>
-    <t>Target 5 x 5 foot area within 45 feet and jump to that location</t>
-  </si>
-  <si>
     <t>Target Ally within 45 feet and pull them adjacent to you.</t>
   </si>
   <si>
@@ -404,6 +386,51 @@
   </si>
   <si>
     <t>4 Charisma, 3 Knowledge</t>
+  </si>
+  <si>
+    <t>Target 5 by 5 foot area within 45 feet and jump to that location</t>
+  </si>
+  <si>
+    <t>6 Spirituality, 1 Finesse</t>
+  </si>
+  <si>
+    <t>Destroy target summon you control. Heal for X life. Return two cards from discard.</t>
+  </si>
+  <si>
+    <t>4 Spirituality, 2 Vigor, 1 Knowledge</t>
+  </si>
+  <si>
+    <t>Roll influence if target is unwilling. Teleport target to a 5 by 5 surface. Exhaust a card.</t>
+  </si>
+  <si>
+    <t>Mark 5 by 5 area. Teleport to target spot no matter the location</t>
+  </si>
+  <si>
+    <t>5 Spirituality, 2 Charisma</t>
+  </si>
+  <si>
+    <t>7 Spirituality</t>
+  </si>
+  <si>
+    <t>Discard a card. Create a 10 by 10 by 10 box over a space. It has 50 hitpoints.</t>
+  </si>
+  <si>
+    <t>7 Charisma</t>
+  </si>
+  <si>
+    <t>1 Craftsmanship, 6 Vigor</t>
+  </si>
+  <si>
+    <t>Increase either an attack die or defense die of one of your equipped weapons, and then decrease an opposite die on thatr weapon. (d4 -&gt; d2, d2 -&gt; 0)</t>
+  </si>
+  <si>
+    <t>7 Craftsmanship</t>
+  </si>
+  <si>
+    <t>4 Perception, 1 Finesse, 2 Knowledge</t>
+  </si>
+  <si>
+    <t>4 Spirituality, 2 Knowledge, 1 Vigor</t>
   </si>
 </sst>
 </file>
@@ -1249,8 +1276,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="220" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1356,7 +1383,7 @@
         <v>25</v>
       </c>
       <c r="N2" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
@@ -1373,7 +1400,7 @@
         <v>28</v>
       </c>
       <c r="E3" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="F3" t="s">
         <v>25</v>
@@ -1397,7 +1424,7 @@
         <v>20</v>
       </c>
       <c r="N3" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
@@ -1414,7 +1441,7 @@
         <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="F4" t="s">
         <v>36</v>
@@ -1432,13 +1459,13 @@
         <v>34</v>
       </c>
       <c r="K4" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="L4" t="s">
         <v>25</v>
       </c>
       <c r="N4" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
@@ -1473,13 +1500,13 @@
         <v>38</v>
       </c>
       <c r="K5" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="L5" t="s">
         <v>25</v>
       </c>
       <c r="N5" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1517,7 +1544,7 @@
         <v>45</v>
       </c>
       <c r="N6" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1534,7 +1561,7 @@
         <v>48</v>
       </c>
       <c r="E7" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
@@ -1552,13 +1579,13 @@
         <v>38</v>
       </c>
       <c r="K7" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="L7" t="s">
         <v>20</v>
       </c>
       <c r="N7" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1572,7 +1599,7 @@
         <v>22</v>
       </c>
       <c r="E8" t="s">
-        <v>116</v>
+        <v>121</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
@@ -1587,13 +1614,13 @@
         <v>22</v>
       </c>
       <c r="K8" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="L8" t="s">
         <v>20</v>
       </c>
       <c r="N8" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1607,10 +1634,10 @@
         <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="E9" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
@@ -1628,13 +1655,13 @@
         <v>38</v>
       </c>
       <c r="K9" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="L9" t="s">
         <v>36</v>
       </c>
       <c r="N9" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
@@ -1663,13 +1690,13 @@
         <v>27</v>
       </c>
       <c r="K10" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
       <c r="L10" t="s">
         <v>36</v>
       </c>
       <c r="N10" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
@@ -1706,6 +1733,9 @@
       <c r="L11" t="s">
         <v>20</v>
       </c>
+      <c r="N11" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -1721,13 +1751,13 @@
         <v>65</v>
       </c>
       <c r="E12" t="s">
-        <v>67</v>
+        <v>123</v>
       </c>
       <c r="F12" t="s">
         <v>25</v>
       </c>
       <c r="G12" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="H12" t="s">
         <v>62</v>
@@ -1736,36 +1766,39 @@
         <v>22</v>
       </c>
       <c r="J12" t="s">
+        <v>68</v>
+      </c>
+      <c r="K12" t="s">
         <v>69</v>
-      </c>
-      <c r="K12" t="s">
-        <v>70</v>
       </c>
       <c r="L12" t="s">
         <v>20</v>
+      </c>
+      <c r="N12" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" t="s">
         <v>71</v>
-      </c>
-      <c r="B13" t="s">
-        <v>72</v>
       </c>
       <c r="C13" t="s">
         <v>22</v>
       </c>
       <c r="D13" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E13" t="s">
-        <v>74</v>
+        <v>125</v>
       </c>
       <c r="F13" t="s">
         <v>20</v>
       </c>
       <c r="G13" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H13" t="s">
         <v>47</v>
@@ -1774,117 +1807,129 @@
         <v>66</v>
       </c>
       <c r="K13" t="s">
-        <v>76</v>
+        <v>126</v>
       </c>
       <c r="L13" t="s">
         <v>25</v>
+      </c>
+      <c r="N13" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>74</v>
+      </c>
+      <c r="E14" t="s">
         <v>78</v>
-      </c>
-      <c r="C14" t="s">
-        <v>77</v>
-      </c>
-      <c r="E14" t="s">
-        <v>82</v>
       </c>
       <c r="F14" t="s">
         <v>20</v>
       </c>
       <c r="G14" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="H14" t="s">
         <v>47</v>
       </c>
       <c r="I14" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="K14" t="s">
-        <v>81</v>
+        <v>129</v>
       </c>
       <c r="L14" t="s">
         <v>20</v>
+      </c>
+      <c r="N14" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
       </c>
       <c r="D15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E15" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>
       </c>
       <c r="G15" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="H15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="I15" t="s">
         <v>22</v>
       </c>
       <c r="J15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="K15" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="L15" t="s">
         <v>20</v>
+      </c>
+      <c r="N15" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
       </c>
       <c r="C16" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="D16" t="s">
         <v>38</v>
       </c>
       <c r="E16" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="F16" t="s">
         <v>25</v>
       </c>
       <c r="G16" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="H16" t="s">
         <v>16</v>
       </c>
       <c r="I16" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="K16" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="L16" t="s">
         <v>20</v>
       </c>
+      <c r="N16" t="s">
+        <v>131</v>
+      </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="B17" t="s">
         <v>16</v>
@@ -1896,16 +1941,16 @@
         <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>93</v>
+        <v>132</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
       </c>
       <c r="G17" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="H17" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="I17" t="s">
         <v>17</v>
@@ -1914,15 +1959,18 @@
         <v>38</v>
       </c>
       <c r="K17" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="L17" t="s">
         <v>20</v>
       </c>
+      <c r="N17" t="s">
+        <v>133</v>
+      </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="B18" t="s">
         <v>30</v>
@@ -1934,13 +1982,13 @@
         <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="F18" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="G18" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="H18" t="s">
         <v>30</v>
@@ -1949,18 +1997,21 @@
         <v>22</v>
       </c>
       <c r="K18" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="L18" t="s">
         <v>25</v>
       </c>
+      <c r="N18" t="s">
+        <v>134</v>
+      </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="B19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C19" t="s">
         <v>22</v>
@@ -1969,13 +2020,13 @@
         <v>28</v>
       </c>
       <c r="E19" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F19" t="s">
         <v>25</v>
       </c>
       <c r="G19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="H19" t="s">
         <v>52</v>
@@ -1987,10 +2038,13 @@
         <v>38</v>
       </c>
       <c r="K19" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="L19" t="s">
         <v>20</v>
+      </c>
+      <c r="N19" t="s">
+        <v>135</v>
       </c>
     </row>
   </sheetData>

</xml_diff>